<commit_message>
Add lawyer init data.
</commit_message>
<xml_diff>
--- a/industry/dsi_lawyer/data/OrgPerson.xlsx
+++ b/industry/dsi_lawyer/data/OrgPerson.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
   <si>
     <t>序号</t>
   </si>
@@ -27,12 +27,18 @@
     <t>上级组织</t>
   </si>
   <si>
+    <t>组织分类</t>
+  </si>
+  <si>
     <t>恩德律师事务所</t>
   </si>
   <si>
     <t>推广组</t>
   </si>
   <si>
+    <t>HR组织</t>
+  </si>
+  <si>
     <t>电话组</t>
   </si>
   <si>
@@ -43,6 +49,9 @@
   </si>
   <si>
     <t>姓名</t>
+  </si>
+  <si>
+    <t>部门</t>
   </si>
   <si>
     <t>账号</t>
@@ -1122,7 +1131,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="4"/>
@@ -1141,7 +1150,9 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:2">
@@ -1149,51 +1160,63 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1208,177 +1231,177 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1393,7 +1416,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="6"/>
@@ -1404,18 +1427,18 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="6:7">
@@ -1423,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="6:7">
@@ -1431,7 +1454,7 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="6:7">
@@ -1439,7 +1462,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="6:7">
@@ -1447,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="6:7">
@@ -1455,7 +1478,7 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>